<commit_message>
completed most of uplift
</commit_message>
<xml_diff>
--- a/Uplift/Uplift Survey.xlsx
+++ b/Uplift/Uplift Survey.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="94">
   <si>
     <t xml:space="preserve">Node</t>
   </si>
@@ -100,6 +100,9 @@
     <t xml:space="preserve">Must be true if named primary researcher</t>
   </si>
   <si>
+    <t xml:space="preserve">Would need to find a way to split out into individual researchers</t>
+  </si>
+  <si>
     <t xml:space="preserve">email</t>
   </si>
   <si>
@@ -142,102 +145,111 @@
     <t xml:space="preserve">Power</t>
   </si>
   <si>
+    <t xml:space="preserve">Minimum effect size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be easily inferred from munum effect size with some regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could only get the MDE string, not uniform enough to extract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subclass of sampling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randomization unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easily inferred from randomisation unit with a data dictionary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stratified</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randomization unit, Experimental design, Randomisation method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will need to search for keywords in these three variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demographic Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be a bit harder to pick out demographic variables due to overlap with clustering level - will need to analysis these fields for common variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AEA Dataset has sampling by treatment arm - may be better than by RCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample size number clusters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easily inferred from whether an entry has been given for the sample size number clusters variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hasNoOfClusters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easily inferred from this variable, will just have to extract number via regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClusterType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have issue with commas and duplicates from regex but is sorting correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treatment Arm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sampleSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move sampling to here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isControl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InterventionTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The intervention is laid out in a body of text, but it may be difficult to categorise into limited types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TreatmentVar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intervention, Outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatmentEffect</t>
+  </si>
+  <si>
     <t xml:space="preserve">float</t>
   </si>
   <si>
-    <t xml:space="preserve">Minimum effect size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should be easily inferred from munum effect size with some regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sampling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Random</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subclass of sampling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Randomization unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easily inferred from randomisation unit with a data dictionary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stratified</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Randomization unit, Experimental design, Randomisation method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Will need to search for keywords in these three variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demographic Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Will be a bit harder to pick out demographic variables due to overlap with clustering level - will need to analysis these fields for common variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AEA Dataset has sampling by treatment arm - may be better than by RCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clustered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample size number clusters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easily inferred from whether an entry has been given for the sample size number clusters variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hasNoOfClusters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easily inferred from this variable, will just have to extract number via regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treatment Arm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intervention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sampleSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move sampling to here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isControl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InterventionTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The intervention is laid out in a body of text, but it may be difficult to categorise into limited types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TreatmentVar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intervention, Outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treatmentEffect</t>
-  </si>
-  <si>
     <t xml:space="preserve">Would likely need to be be inferred from the source paper in most instances, difficult to choose which coefficient is the important one in an automated way</t>
   </si>
   <si>
@@ -263,9 +275,6 @@
   </si>
   <si>
     <t xml:space="preserve">Slightly more complicated extraction but possible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place</t>
   </si>
   <si>
     <t xml:space="preserve">Timespan</t>
@@ -411,7 +420,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,6 +442,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,13 +530,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.83"/>
@@ -531,7 +544,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="55.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
@@ -574,8 +587,9 @@
       <c r="F2" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -586,6 +600,7 @@
       <c r="F3" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -622,7 +637,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -633,6 +648,7 @@
       <c r="F6" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -664,13 +680,17 @@
       <c r="G8" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3"/>
       <c r="E9" s="0" t="s">
@@ -680,16 +700,16 @@
         <v>21</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3"/>
       <c r="E10" s="0" t="s">
@@ -699,16 +719,16 @@
         <v>21</v>
       </c>
       <c r="G10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C11" s="4"/>
       <c r="E11" s="0" t="s">
@@ -718,385 +738,416 @@
         <v>21</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1"/>
       <c r="F12" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4"/>
       <c r="E13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3"/>
       <c r="E14" s="0" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="1"/>
       <c r="F15" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3"/>
       <c r="E16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="4"/>
       <c r="E18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3"/>
       <c r="E19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3"/>
       <c r="E20" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="E21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="F22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="F21" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="H22" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="C23" s="3"/>
+      <c r="H23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="E25" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="E24" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="E25" s="0" t="s">
-        <v>69</v>
-      </c>
       <c r="F25" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="0" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="E26" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C27" s="5"/>
       <c r="E27" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G27" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="E28" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="E28" s="0" t="s">
+      <c r="F28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="0" t="s">
+      <c r="H28" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>79</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="7"/>
       <c r="E29" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="7"/>
       <c r="E30" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>77</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1"/>
       <c r="F31" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="C32" s="7"/>
       <c r="D32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="G32" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>84</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1"/>
       <c r="F34" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
+        <v>93</v>
+      </c>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>